<commit_message>
Add 2 more parts to Task 2 validation
</commit_message>
<xml_diff>
--- a/REopt Julia Package Scripts/results/results_emissions_reductions.xlsx
+++ b/REopt Julia Package Scripts/results/results_emissions_reductions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbernal\Documents\GitHub\REopt-Analysis-Scripts\REopt Julia Package Scripts\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE11670B-11E2-4FBB-91E0-B7FB16C16489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED60FE43-A846-4CB8-A596-013167386A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="23" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="30" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resultsA_0" sheetId="2" r:id="rId1"/>
@@ -42,6 +42,15 @@
     <sheet name="Task2.PartB" sheetId="26" r:id="rId27"/>
     <sheet name="Task2.PartC" sheetId="37" r:id="rId28"/>
     <sheet name="resultsA_11" sheetId="38" r:id="rId29"/>
+    <sheet name="Task2.PartA(updated)" sheetId="39" r:id="rId30"/>
+    <sheet name="Task2.PartB(updated)" sheetId="40" r:id="rId31"/>
+    <sheet name="Task2.PartC(updated)" sheetId="41" r:id="rId32"/>
+    <sheet name="Sheet1" sheetId="42" r:id="rId33"/>
+    <sheet name="resultsA_13" sheetId="43" r:id="rId34"/>
+    <sheet name="resultsB_9" sheetId="44" r:id="rId35"/>
+    <sheet name="resultsC_4" sheetId="45" r:id="rId36"/>
+    <sheet name="resultsD_0" sheetId="46" r:id="rId37"/>
+    <sheet name="resultsE_0" sheetId="47" r:id="rId38"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="69">
   <si>
     <t>City</t>
   </si>
@@ -646,14 +655,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819D8DAD-F8DA-4049-BDD4-9E95A2AA356E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E5CC17-B141-44A5-BA2E-6CF70CEC85C0}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -670,7 +679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -687,7 +696,7 @@
         <v>-1.79</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -704,7 +713,7 @@
         <v>-0.87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -721,7 +730,7 @@
         <v>-2.1800000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -744,19 +753,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47CB6FD3-6987-40B1-BFD3-E9AF25E4B236}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F0E04B3-1953-4A26-8F17-0C4F74FC320C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -814,7 +823,7 @@
         <v>-2741986.6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -843,7 +852,7 @@
         <v>-2296535.7799999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -872,7 +881,7 @@
         <v>-2543875.48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -907,19 +916,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FCE439-8F9B-46D4-96D0-C7E65D725A28}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A2F28E-D7EB-4C7B-A061-C45DB9F947F9}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -948,7 +957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -977,7 +986,7 @@
         <v>-8339592.2800000003</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1006,7 +1015,7 @@
         <v>-15742760.09</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>-27788443.390000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1070,24 +1079,24 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456C85A6-F23C-4767-8C95-09CEB66AE27E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C74E42-CF8F-4833-B816-80FDE0EA2431}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" customWidth="1"/>
-    <col min="8" max="8" width="14.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1139,7 +1148,7 @@
         <v>-66.068299999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1174,7 @@
         <v>-140.63720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1191,7 +1200,7 @@
         <v>-52.133899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1223,25 +1232,25 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8906ACEC-52F1-46F0-A33E-DB54292BBD2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46464B32-9966-41FB-B891-ED5257C75E68}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" customWidth="1"/>
-    <col min="9" max="9" width="16.90625" customWidth="1"/>
-    <col min="10" max="10" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1273,7 +1282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1305,7 +1314,7 @@
         <v>-2741986.6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1337,7 +1346,7 @@
         <v>-2296535.7799999998</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1369,7 +1378,7 @@
         <v>-2543875.48</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1407,23 +1416,23 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BE2E53-BB6C-4C2B-8B6A-F0787B138FDE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD5C78A-01CA-4B1A-A0F8-6B716F0A9BD7}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1455,7 +1464,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1487,7 +1496,7 @@
         <v>-8339592.2800000003</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1528,7 @@
         <v>-15742760.09</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1551,7 +1560,7 @@
         <v>-27788443.390000001</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1589,26 +1598,26 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6650DA29-7B4E-4DE9-8A79-665AE955E420}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A4004C-0761-4D04-AA65-EA5FF4400B2B}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" customWidth="1"/>
-    <col min="9" max="9" width="11.6328125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1690,7 +1699,7 @@
         <v>-66.068299999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1731,7 +1740,7 @@
         <v>-140.63720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1772,7 +1781,7 @@
         <v>-52.133899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1819,29 +1828,29 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD410DD7-D6B2-4568-BBAE-F66A31813E2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B806DA9A-15FF-434D-8B79-9BA58FE538DA}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="6" max="6" width="12.90625" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1888,7 +1897,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1935,7 +1944,7 @@
         <v>-66.068299999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1982,7 +1991,7 @@
         <v>-140.63720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2029,7 +2038,7 @@
         <v>-52.133899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2082,28 +2091,28 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC23619-95FF-4DA4-BD89-3C9DCCC3CB54}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46207520-09D9-44A5-B2F2-4FF0C7FF80FF}">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
     <col min="10" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2153,7 +2162,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2203,7 +2212,7 @@
         <v>-66.068299999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2253,7 +2262,7 @@
         <v>-140.63720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2303,7 +2312,7 @@
         <v>-52.133899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2359,24 +2368,24 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792E3B8F-8488-41F6-A3F7-5E3001D4DDA2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6911B4C3-E22E-4042-9189-7B2C95C5BAC1}">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2426,7 +2435,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2476,7 +2485,7 @@
         <v>-66.068299999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2526,7 +2535,7 @@
         <v>-140.63720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2576,7 +2585,7 @@
         <v>-52.133899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2632,22 +2641,22 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3304C09-35B5-4893-B79A-160D6813C976}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388C3CE0-0669-4314-AFC5-4EE715BD31CC}">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2697,7 +2706,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2747,7 +2756,7 @@
         <v>-66.068299999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2797,7 +2806,7 @@
         <v>-140.63720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2847,7 +2856,7 @@
         <v>-52.133899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2903,14 +2912,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06CEC1D-F378-446B-9C92-3A7539D959FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59988D1F-F5F2-406F-9F49-E57316169A0B}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2936,7 +2945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2962,7 +2971,7 @@
         <v>-2741986.6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2988,7 +2997,7 @@
         <v>-2296535.7799999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3014,7 +3023,7 @@
         <v>-2543875.48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3046,23 +3055,23 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80ACF362-4420-47CC-81DF-7996F1649433}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0464E7A-A67E-4AD3-B640-577834F3FB49}">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3112,7 +3121,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3162,7 +3171,7 @@
         <v>-66.068299999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3212,7 +3221,7 @@
         <v>-140.63720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3262,7 +3271,7 @@
         <v>-52.133899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3318,25 +3327,25 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14046369-96A6-4BA3-A703-1641F26333CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33F064F-3481-4806-B281-D47CE2E8773D}">
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3401,7 +3410,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3466,7 +3475,7 @@
         <v>-2741986.6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3531,7 +3540,7 @@
         <v>-2296535.7799999998</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3596,7 +3605,7 @@
         <v>-2543875.48</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3667,26 +3676,26 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DD74E2-C251-4587-AE29-1AF5B974D794}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE02B12-06CC-4E2C-9B89-B262F460C272}">
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
     <col min="8" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3751,7 +3760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3816,7 +3825,7 @@
         <v>-2898368.32</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3881,7 +3890,7 @@
         <v>-2400831.2799999998</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3946,7 +3955,7 @@
         <v>-2653831.7799999998</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4011,7 +4020,7 @@
         <v>-2022109.01</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>46</v>
       </c>
@@ -4019,7 +4028,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>47</v>
       </c>
@@ -4030,25 +4039,25 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326AC5D7-C0C0-4D40-9B24-DD8C831E61F9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF42B19-CBA1-446B-83C7-7036DE7E6A96}">
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
     <col min="8" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4113,7 +4122,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4178,7 +4187,7 @@
         <v>-2898368.32</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4243,7 +4252,7 @@
         <v>-2400831.2799999998</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4308,7 +4317,7 @@
         <v>-2653831.7799999998</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4373,7 +4382,7 @@
         <v>-2022109.01</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>45</v>
       </c>
@@ -4381,7 +4390,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>41</v>
       </c>
@@ -4392,25 +4401,25 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E649695-D326-429C-BFF0-A7D11AABCF74}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A410E43-4032-47FE-A75C-D883ACAD4215}">
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
     <col min="8" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4475,7 +4484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4540,7 +4549,7 @@
         <v>-2262751.19</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4605,7 +4614,7 @@
         <v>-1956426.15</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4670,7 +4679,7 @@
         <v>-2188156.2599999998</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -4735,7 +4744,7 @@
         <v>-1666408.9</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>44</v>
       </c>
@@ -4746,7 +4755,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>41</v>
       </c>
@@ -4757,25 +4766,25 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4074B42D-6C83-4F91-95FF-774B95991ADE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8483A42-A3E3-4D06-9FDA-6DB46AF57B01}">
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4840,7 +4849,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4905,7 +4914,7 @@
         <v>-2262751.19</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4970,7 +4979,7 @@
         <v>-1956426.15</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5035,7 +5044,7 @@
         <v>-2188156.2599999998</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -5100,7 +5109,7 @@
         <v>-1666408.9</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>37</v>
       </c>
@@ -5111,7 +5120,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>39</v>
       </c>
@@ -5122,24 +5131,24 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECA3C32-DF56-4289-A426-342B6D931157}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09709B2E-1F2B-4D92-845D-0EFB23A64E1C}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5192,7 +5201,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5245,7 +5254,7 @@
         <v>-6274160.2400000002</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5298,7 +5307,7 @@
         <v>-6588757.2300000004</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5351,7 +5360,7 @@
         <v>-6013617.0599999996</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -5404,7 +5413,7 @@
         <v>-7504886.7199999997</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -5460,24 +5469,24 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52197F96-67E8-4EB0-B281-FCD4B17D4E9B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79911F1-691E-456C-A926-FA94D74694DF}">
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5542,7 +5551,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -5607,7 +5616,7 @@
         <v>-2741986.6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5672,7 +5681,7 @@
         <v>-2296535.7799999998</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5737,7 +5746,7 @@
         <v>-2543875.48</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -5802,7 +5811,7 @@
         <v>-1937771.89</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>33</v>
       </c>
@@ -5818,7 +5827,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E8" s="10">
         <f t="shared" ref="E8:E10" si="0">E3-C3</f>
         <v>240577</v>
@@ -5831,7 +5840,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E9" s="10">
         <f t="shared" si="0"/>
         <v>-37482</v>
@@ -5844,7 +5853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E10" s="10">
         <f t="shared" si="0"/>
         <v>-35597</v>
@@ -5860,23 +5869,23 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48604EE7-9ACD-4EA7-80AF-90D37934F1DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F823FD4-FBA8-4795-9EBE-F8B53B393B5B}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5941,7 +5950,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6006,7 +6015,7 @@
         <v>-8339592.2800000003</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6071,7 +6080,7 @@
         <v>-15742760.09</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -6136,7 +6145,7 @@
         <v>-27788443.390000001</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -6207,14 +6216,14 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D0CE07-9755-4158-8BA7-42B6A286D6A5}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6267,7 +6276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6320,7 +6329,7 @@
         <v>-6274160.2400000002</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6373,7 +6382,7 @@
         <v>-6588757.2300000004</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -6426,7 +6435,7 @@
         <v>-6013617.0599999996</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -6485,14 +6494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474C4736-3D75-4B93-9A82-A147035D0674}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F0D380-99E8-4AAF-B31E-87BD72B59A17}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6518,7 +6527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6544,7 +6553,7 @@
         <v>-8339592.2800000003</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6570,7 +6579,7 @@
         <v>-15742760.09</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -6596,7 +6605,7 @@
         <v>-27788443.390000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -6620,6 +6629,2635 @@
       </c>
       <c r="H5">
         <v>-86975102.640000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D8DEE0-EF16-473D-BC77-801E00279EC5}">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6">
+        <v>13614485</v>
+      </c>
+      <c r="C2" s="6">
+        <v>13614484</v>
+      </c>
+      <c r="D2" s="6">
+        <v>45990</v>
+      </c>
+      <c r="E2" s="6">
+        <v>45990</v>
+      </c>
+      <c r="F2" s="6">
+        <v>61320</v>
+      </c>
+      <c r="G2" s="6">
+        <v>61320</v>
+      </c>
+      <c r="H2" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I2" s="6">
+        <v>9873.9500000000007</v>
+      </c>
+      <c r="J2" s="6">
+        <v>9873.9500000000007</v>
+      </c>
+      <c r="K2" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="L2" s="6">
+        <v>212486.08</v>
+      </c>
+      <c r="M2" s="6">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>-1.61</v>
+      </c>
+      <c r="P2" s="2">
+        <v>-65.965999999999994</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>-5661648.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>13614485</v>
+      </c>
+      <c r="C3" s="6">
+        <v>13614484</v>
+      </c>
+      <c r="D3" s="6">
+        <v>45990</v>
+      </c>
+      <c r="E3" s="6">
+        <v>45990</v>
+      </c>
+      <c r="F3" s="6">
+        <v>61320</v>
+      </c>
+      <c r="G3" s="6">
+        <v>61320</v>
+      </c>
+      <c r="H3" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I3" s="6">
+        <v>6624.5</v>
+      </c>
+      <c r="J3" s="6">
+        <v>6624.5</v>
+      </c>
+      <c r="K3" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="L3" s="6">
+        <v>142558.26</v>
+      </c>
+      <c r="M3" s="6">
+        <v>81287.350000000006</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>-0.75</v>
+      </c>
+      <c r="P3" s="2">
+        <v>-143.76650000000001</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>-5853986.5099999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>13614485</v>
+      </c>
+      <c r="C4" s="6">
+        <v>13614484</v>
+      </c>
+      <c r="D4" s="6">
+        <v>45990</v>
+      </c>
+      <c r="E4" s="6">
+        <v>45990</v>
+      </c>
+      <c r="F4" s="6">
+        <v>61320</v>
+      </c>
+      <c r="G4" s="6">
+        <v>61320</v>
+      </c>
+      <c r="H4" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I4" s="6">
+        <v>11250.64</v>
+      </c>
+      <c r="J4" s="6">
+        <v>11250.64</v>
+      </c>
+      <c r="K4" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="L4" s="6">
+        <v>242112.23</v>
+      </c>
+      <c r="M4" s="6">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>-1.98</v>
+      </c>
+      <c r="P4" s="2">
+        <v>-52.238799999999998</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>-5481819.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>13614485</v>
+      </c>
+      <c r="C5" s="6">
+        <v>13614484</v>
+      </c>
+      <c r="D5" s="6">
+        <v>45990</v>
+      </c>
+      <c r="E5" s="6">
+        <v>45990</v>
+      </c>
+      <c r="F5" s="6">
+        <v>61320</v>
+      </c>
+      <c r="G5" s="6">
+        <v>61320</v>
+      </c>
+      <c r="H5" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I5" s="6">
+        <v>6675.22</v>
+      </c>
+      <c r="J5" s="6">
+        <v>6675.22</v>
+      </c>
+      <c r="K5" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="L5" s="6">
+        <v>143649.88</v>
+      </c>
+      <c r="M5" s="6">
+        <v>81287.350000000006</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>-0.77</v>
+      </c>
+      <c r="P5" s="2">
+        <v>-163.7116</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>-6781392.29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066A1629-0143-4A7A-8CD7-19FA617005BB}">
+  <dimension ref="A1:U5"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6">
+        <v>8532</v>
+      </c>
+      <c r="C2" s="6">
+        <v>10218393</v>
+      </c>
+      <c r="D2" s="6">
+        <v>18193</v>
+      </c>
+      <c r="E2" s="6">
+        <v>13614485</v>
+      </c>
+      <c r="F2" s="6">
+        <v>5624132</v>
+      </c>
+      <c r="G2" s="6">
+        <v>45990</v>
+      </c>
+      <c r="H2" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I2" s="6">
+        <v>61320</v>
+      </c>
+      <c r="J2" s="6">
+        <v>61320</v>
+      </c>
+      <c r="K2" s="6">
+        <v>45990</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>2832.99</v>
+      </c>
+      <c r="N2" s="6">
+        <v>2832.99</v>
+      </c>
+      <c r="O2" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="P2" s="6">
+        <v>60965.52</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>1528.6206999999999</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="U2" s="2">
+        <v>-18212119.960000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>5317</v>
+      </c>
+      <c r="C3" s="6">
+        <v>6245185</v>
+      </c>
+      <c r="D3" s="6">
+        <v>7473</v>
+      </c>
+      <c r="E3" s="6">
+        <v>13614485</v>
+      </c>
+      <c r="F3" s="6">
+        <v>8262935</v>
+      </c>
+      <c r="G3" s="6">
+        <v>45990</v>
+      </c>
+      <c r="H3" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I3" s="6">
+        <v>61320</v>
+      </c>
+      <c r="J3" s="6">
+        <v>61320</v>
+      </c>
+      <c r="K3" s="6">
+        <v>45990</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6">
+        <v>2832.99</v>
+      </c>
+      <c r="N3" s="6">
+        <v>2832.99</v>
+      </c>
+      <c r="O3" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="P3" s="6">
+        <v>60965.51</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>81287.350000000006</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>957.24980000000005</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="U3" s="2">
+        <v>-11404757.710000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
+        <v>8200</v>
+      </c>
+      <c r="C4" s="6">
+        <v>10811776</v>
+      </c>
+      <c r="D4" s="6">
+        <v>19889</v>
+      </c>
+      <c r="E4" s="6">
+        <v>13614485</v>
+      </c>
+      <c r="F4" s="6">
+        <v>4607425</v>
+      </c>
+      <c r="G4" s="6">
+        <v>45990</v>
+      </c>
+      <c r="H4" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I4" s="6">
+        <v>61320</v>
+      </c>
+      <c r="J4" s="6">
+        <v>61320</v>
+      </c>
+      <c r="K4" s="6">
+        <v>45990</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>2832.99</v>
+      </c>
+      <c r="N4" s="6">
+        <v>2832.99</v>
+      </c>
+      <c r="O4" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="P4" s="6">
+        <v>60965.52</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>1542.4716000000001</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="U4" s="2">
+        <v>-18377140.969999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5664</v>
+      </c>
+      <c r="C5" s="6">
+        <v>8069281</v>
+      </c>
+      <c r="D5" s="6">
+        <v>9967</v>
+      </c>
+      <c r="E5" s="6">
+        <v>13614485</v>
+      </c>
+      <c r="F5" s="6">
+        <v>6963924</v>
+      </c>
+      <c r="G5" s="6">
+        <v>45990</v>
+      </c>
+      <c r="H5" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I5" s="6">
+        <v>61320</v>
+      </c>
+      <c r="J5" s="6">
+        <v>61320</v>
+      </c>
+      <c r="K5" s="6">
+        <v>45990</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>2832.99</v>
+      </c>
+      <c r="N5" s="6">
+        <v>2832.99</v>
+      </c>
+      <c r="O5" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="P5" s="6">
+        <v>60965.51</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>81287.350000000006</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>1049.8194000000001</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="U5" s="2">
+        <v>-12507639.51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB7D02C-3F76-4591-862E-785FB513EB34}">
+  <dimension ref="A1:U5"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6">
+        <v>3071</v>
+      </c>
+      <c r="C2" s="6">
+        <v>3677688</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>3404304</v>
+      </c>
+      <c r="F2" s="6">
+        <v>4761</v>
+      </c>
+      <c r="G2" s="6">
+        <v>11500</v>
+      </c>
+      <c r="H2" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I2" s="6">
+        <v>61320</v>
+      </c>
+      <c r="J2" s="6">
+        <v>61320</v>
+      </c>
+      <c r="K2" s="6">
+        <v>45990</v>
+      </c>
+      <c r="L2" s="6">
+        <v>45987</v>
+      </c>
+      <c r="M2" s="6">
+        <v>2438.65</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0.19</v>
+      </c>
+      <c r="O2" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="P2" s="6">
+        <v>60965.52</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R2" s="6">
+        <v>60961.43</v>
+      </c>
+      <c r="S2" s="2">
+        <v>210.85130000000001</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="U2" s="2">
+        <v>-2701022.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6">
+        <v>7115</v>
+      </c>
+      <c r="C3" s="6">
+        <v>8521096</v>
+      </c>
+      <c r="D3" s="6">
+        <v>11514</v>
+      </c>
+      <c r="E3" s="6">
+        <v>6807692</v>
+      </c>
+      <c r="F3" s="6">
+        <v>3137</v>
+      </c>
+      <c r="G3" s="6">
+        <v>22997</v>
+      </c>
+      <c r="H3" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I3" s="6">
+        <v>61320</v>
+      </c>
+      <c r="J3" s="6">
+        <v>61320</v>
+      </c>
+      <c r="K3" s="6">
+        <v>45990</v>
+      </c>
+      <c r="L3" s="6">
+        <v>30658</v>
+      </c>
+      <c r="M3" s="6">
+        <v>1625.76</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.13</v>
+      </c>
+      <c r="O3" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="P3" s="6">
+        <v>40643.68</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R3" s="6">
+        <v>40640.980000000003</v>
+      </c>
+      <c r="S3" s="2">
+        <v>420.29660000000001</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="U3" s="2">
+        <v>-10768134.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6">
+        <v>11644</v>
+      </c>
+      <c r="C4" s="6">
+        <v>13945476</v>
+      </c>
+      <c r="D4" s="6">
+        <v>25145</v>
+      </c>
+      <c r="E4" s="6">
+        <v>10211400</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3730</v>
+      </c>
+      <c r="G4" s="6">
+        <v>34494</v>
+      </c>
+      <c r="H4" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I4" s="6">
+        <v>61320</v>
+      </c>
+      <c r="J4" s="6">
+        <v>61320</v>
+      </c>
+      <c r="K4" s="6">
+        <v>45990</v>
+      </c>
+      <c r="L4" s="6">
+        <v>15328</v>
+      </c>
+      <c r="M4" s="6">
+        <v>812.89</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="O4" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="P4" s="6">
+        <v>20321.84</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R4" s="6">
+        <v>20318.63</v>
+      </c>
+      <c r="S4" s="2">
+        <v>591.48199999999997</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="U4" s="2">
+        <v>-22730981.510000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6">
+        <v>35019</v>
+      </c>
+      <c r="C5" s="6">
+        <v>41940634</v>
+      </c>
+      <c r="D5" s="6">
+        <v>113618</v>
+      </c>
+      <c r="E5" s="6">
+        <v>13614485</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>45990</v>
+      </c>
+      <c r="H5" s="6">
+        <v>45990</v>
+      </c>
+      <c r="I5" s="6">
+        <v>61320</v>
+      </c>
+      <c r="J5" s="6">
+        <v>61320</v>
+      </c>
+      <c r="K5" s="6">
+        <v>45990</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6">
+        <v>3251.49</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>1586.3235999999999</v>
+      </c>
+      <c r="T5" s="3">
+        <v>1</v>
+      </c>
+      <c r="U5" s="2">
+        <v>-81284720.049999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58095AC6-462D-44BB-9085-4E6C0C8A4690}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F347DE27-2FC5-4E70-81B0-3FA9AF072673}">
+  <dimension ref="A1:Q5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>13614485</v>
+      </c>
+      <c r="C2">
+        <v>13614484</v>
+      </c>
+      <c r="D2">
+        <v>45990</v>
+      </c>
+      <c r="E2">
+        <v>45990</v>
+      </c>
+      <c r="F2">
+        <v>61320</v>
+      </c>
+      <c r="G2">
+        <v>61320</v>
+      </c>
+      <c r="H2">
+        <v>45990</v>
+      </c>
+      <c r="I2">
+        <v>9873.9500000000007</v>
+      </c>
+      <c r="J2">
+        <v>9873.9500000000007</v>
+      </c>
+      <c r="K2">
+        <v>3251.49</v>
+      </c>
+      <c r="L2">
+        <v>212486.08</v>
+      </c>
+      <c r="M2">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>-1.61</v>
+      </c>
+      <c r="P2">
+        <v>-65.965999999999994</v>
+      </c>
+      <c r="Q2">
+        <v>-5661648.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>13614485</v>
+      </c>
+      <c r="C3">
+        <v>13614484</v>
+      </c>
+      <c r="D3">
+        <v>45990</v>
+      </c>
+      <c r="E3">
+        <v>45990</v>
+      </c>
+      <c r="F3">
+        <v>61320</v>
+      </c>
+      <c r="G3">
+        <v>61320</v>
+      </c>
+      <c r="H3">
+        <v>45990</v>
+      </c>
+      <c r="I3">
+        <v>6624.5</v>
+      </c>
+      <c r="J3">
+        <v>6624.5</v>
+      </c>
+      <c r="K3">
+        <v>3251.49</v>
+      </c>
+      <c r="L3">
+        <v>142558.26</v>
+      </c>
+      <c r="M3">
+        <v>81287.350000000006</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>-0.75</v>
+      </c>
+      <c r="P3">
+        <v>-143.76650000000001</v>
+      </c>
+      <c r="Q3">
+        <v>-5853986.5099999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>13614485</v>
+      </c>
+      <c r="C4">
+        <v>13614484</v>
+      </c>
+      <c r="D4">
+        <v>45990</v>
+      </c>
+      <c r="E4">
+        <v>45990</v>
+      </c>
+      <c r="F4">
+        <v>61320</v>
+      </c>
+      <c r="G4">
+        <v>61320</v>
+      </c>
+      <c r="H4">
+        <v>45990</v>
+      </c>
+      <c r="I4">
+        <v>11250.64</v>
+      </c>
+      <c r="J4">
+        <v>11250.64</v>
+      </c>
+      <c r="K4">
+        <v>3251.49</v>
+      </c>
+      <c r="L4">
+        <v>242112.23</v>
+      </c>
+      <c r="M4">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>-1.98</v>
+      </c>
+      <c r="P4">
+        <v>-52.238799999999998</v>
+      </c>
+      <c r="Q4">
+        <v>-5481819.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>13614485</v>
+      </c>
+      <c r="C5">
+        <v>13614484</v>
+      </c>
+      <c r="D5">
+        <v>45990</v>
+      </c>
+      <c r="E5">
+        <v>45990</v>
+      </c>
+      <c r="F5">
+        <v>61320</v>
+      </c>
+      <c r="G5">
+        <v>61320</v>
+      </c>
+      <c r="H5">
+        <v>45990</v>
+      </c>
+      <c r="I5">
+        <v>6675.22</v>
+      </c>
+      <c r="J5">
+        <v>6675.22</v>
+      </c>
+      <c r="K5">
+        <v>3251.49</v>
+      </c>
+      <c r="L5">
+        <v>143649.88</v>
+      </c>
+      <c r="M5">
+        <v>81287.350000000006</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>-0.77</v>
+      </c>
+      <c r="P5">
+        <v>-163.7116</v>
+      </c>
+      <c r="Q5">
+        <v>-6781392.29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CE4750-2F69-4734-9754-85A94DAF32A1}">
+  <dimension ref="A1:U5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>8986</v>
+      </c>
+      <c r="C2">
+        <v>10761435</v>
+      </c>
+      <c r="D2">
+        <v>19160</v>
+      </c>
+      <c r="E2">
+        <v>14338009</v>
+      </c>
+      <c r="F2">
+        <v>5923019</v>
+      </c>
+      <c r="G2">
+        <v>48434</v>
+      </c>
+      <c r="H2">
+        <v>48434</v>
+      </c>
+      <c r="I2">
+        <v>64579</v>
+      </c>
+      <c r="J2">
+        <v>64579</v>
+      </c>
+      <c r="K2">
+        <v>48434</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>2983.54</v>
+      </c>
+      <c r="N2">
+        <v>2983.54</v>
+      </c>
+      <c r="O2">
+        <v>3424.29</v>
+      </c>
+      <c r="P2">
+        <v>64205.45</v>
+      </c>
+      <c r="Q2">
+        <v>85607.26</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>1528.6038000000001</v>
+      </c>
+      <c r="T2">
+        <v>0.25</v>
+      </c>
+      <c r="U2">
+        <v>-19179977.829999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>5600</v>
+      </c>
+      <c r="C3">
+        <v>6577077</v>
+      </c>
+      <c r="D3">
+        <v>7871</v>
+      </c>
+      <c r="E3">
+        <v>14338009</v>
+      </c>
+      <c r="F3">
+        <v>8702057</v>
+      </c>
+      <c r="G3">
+        <v>48434</v>
+      </c>
+      <c r="H3">
+        <v>48434</v>
+      </c>
+      <c r="I3">
+        <v>64579</v>
+      </c>
+      <c r="J3">
+        <v>64579</v>
+      </c>
+      <c r="K3">
+        <v>48434</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>2983.54</v>
+      </c>
+      <c r="N3">
+        <v>2983.54</v>
+      </c>
+      <c r="O3">
+        <v>3424.29</v>
+      </c>
+      <c r="P3">
+        <v>64205.440000000002</v>
+      </c>
+      <c r="Q3">
+        <v>85607.26</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>957.23929999999996</v>
+      </c>
+      <c r="T3">
+        <v>0.25</v>
+      </c>
+      <c r="U3">
+        <v>-12010847.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>8371</v>
+      </c>
+      <c r="C4">
+        <v>11036987</v>
+      </c>
+      <c r="D4">
+        <v>20304</v>
+      </c>
+      <c r="E4">
+        <v>13898073</v>
+      </c>
+      <c r="F4">
+        <v>4703399</v>
+      </c>
+      <c r="G4">
+        <v>46948</v>
+      </c>
+      <c r="H4">
+        <v>46948</v>
+      </c>
+      <c r="I4">
+        <v>62597</v>
+      </c>
+      <c r="J4">
+        <v>62597</v>
+      </c>
+      <c r="K4">
+        <v>46948</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>2892</v>
+      </c>
+      <c r="N4">
+        <v>2892</v>
+      </c>
+      <c r="O4">
+        <v>3319.22</v>
+      </c>
+      <c r="P4">
+        <v>62235.44</v>
+      </c>
+      <c r="Q4">
+        <v>82980.59</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1542.4668999999999</v>
+      </c>
+      <c r="T4">
+        <v>0.25</v>
+      </c>
+      <c r="U4">
+        <v>-18759940.350000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>5831</v>
+      </c>
+      <c r="C5">
+        <v>8307281</v>
+      </c>
+      <c r="D5">
+        <v>10261</v>
+      </c>
+      <c r="E5">
+        <v>14016035</v>
+      </c>
+      <c r="F5">
+        <v>7169322</v>
+      </c>
+      <c r="G5">
+        <v>47346</v>
+      </c>
+      <c r="H5">
+        <v>47346</v>
+      </c>
+      <c r="I5">
+        <v>63129</v>
+      </c>
+      <c r="J5">
+        <v>63129</v>
+      </c>
+      <c r="K5">
+        <v>47346</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>2916.55</v>
+      </c>
+      <c r="N5">
+        <v>2916.55</v>
+      </c>
+      <c r="O5">
+        <v>3347.4</v>
+      </c>
+      <c r="P5">
+        <v>62763.66</v>
+      </c>
+      <c r="Q5">
+        <v>83684.88</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1049.8236999999999</v>
+      </c>
+      <c r="T5">
+        <v>0.25</v>
+      </c>
+      <c r="U5">
+        <v>-12876546.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D86512-FC94-4E8E-B295-0E56CBC11F30}">
+  <dimension ref="A1:U5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>8532</v>
+      </c>
+      <c r="C2">
+        <v>10218393</v>
+      </c>
+      <c r="D2">
+        <v>18193</v>
+      </c>
+      <c r="E2">
+        <v>13614485</v>
+      </c>
+      <c r="F2">
+        <v>5624132</v>
+      </c>
+      <c r="G2">
+        <v>45990</v>
+      </c>
+      <c r="H2">
+        <v>45990</v>
+      </c>
+      <c r="I2">
+        <v>61320</v>
+      </c>
+      <c r="J2">
+        <v>61320</v>
+      </c>
+      <c r="K2">
+        <v>45990</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>2832.99</v>
+      </c>
+      <c r="N2">
+        <v>2832.99</v>
+      </c>
+      <c r="O2">
+        <v>3251.49</v>
+      </c>
+      <c r="P2">
+        <v>60965.52</v>
+      </c>
+      <c r="Q2">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>1528.6206999999999</v>
+      </c>
+      <c r="T2">
+        <v>0.25</v>
+      </c>
+      <c r="U2">
+        <v>-18212119.960000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>10803</v>
+      </c>
+      <c r="C3">
+        <v>12937831</v>
+      </c>
+      <c r="D3">
+        <v>24272</v>
+      </c>
+      <c r="E3">
+        <v>13614485</v>
+      </c>
+      <c r="F3">
+        <v>3952540</v>
+      </c>
+      <c r="G3">
+        <v>45990</v>
+      </c>
+      <c r="H3">
+        <v>45990</v>
+      </c>
+      <c r="I3">
+        <v>61320</v>
+      </c>
+      <c r="J3">
+        <v>61320</v>
+      </c>
+      <c r="K3">
+        <v>45990</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1888.66</v>
+      </c>
+      <c r="N3">
+        <v>1888.66</v>
+      </c>
+      <c r="O3">
+        <v>3251.49</v>
+      </c>
+      <c r="P3">
+        <v>40643.68</v>
+      </c>
+      <c r="Q3">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>849.95479999999998</v>
+      </c>
+      <c r="T3">
+        <v>0.5</v>
+      </c>
+      <c r="U3">
+        <v>-21268452.420000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>16459</v>
+      </c>
+      <c r="C4">
+        <v>19712511</v>
+      </c>
+      <c r="D4">
+        <v>32628</v>
+      </c>
+      <c r="E4">
+        <v>13614485</v>
+      </c>
+      <c r="F4">
+        <v>2068988</v>
+      </c>
+      <c r="G4">
+        <v>45990</v>
+      </c>
+      <c r="H4">
+        <v>45990</v>
+      </c>
+      <c r="I4">
+        <v>61320</v>
+      </c>
+      <c r="J4">
+        <v>61320</v>
+      </c>
+      <c r="K4">
+        <v>45990</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>944.33</v>
+      </c>
+      <c r="N4">
+        <v>944.33</v>
+      </c>
+      <c r="O4">
+        <v>3251.49</v>
+      </c>
+      <c r="P4">
+        <v>20321.84</v>
+      </c>
+      <c r="Q4">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>843.11869999999999</v>
+      </c>
+      <c r="T4">
+        <v>0.75</v>
+      </c>
+      <c r="U4">
+        <v>-32149796.210000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>35019</v>
+      </c>
+      <c r="C5">
+        <v>41940634</v>
+      </c>
+      <c r="D5">
+        <v>113618</v>
+      </c>
+      <c r="E5">
+        <v>13614485</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>45990</v>
+      </c>
+      <c r="H5">
+        <v>45990</v>
+      </c>
+      <c r="I5">
+        <v>61320</v>
+      </c>
+      <c r="J5">
+        <v>61320</v>
+      </c>
+      <c r="K5">
+        <v>45990</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>3251.49</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1586.3235999999999</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>-81284720.049999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF05BFBD-BC20-4771-9B7C-77B617057DDC}">
+  <dimension ref="A1:U5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3234</v>
+      </c>
+      <c r="C2">
+        <v>3873134</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>3585221</v>
+      </c>
+      <c r="F2">
+        <v>5014</v>
+      </c>
+      <c r="G2">
+        <v>12111</v>
+      </c>
+      <c r="H2">
+        <v>48434</v>
+      </c>
+      <c r="I2">
+        <v>64579</v>
+      </c>
+      <c r="J2">
+        <v>64579</v>
+      </c>
+      <c r="K2">
+        <v>48434</v>
+      </c>
+      <c r="L2">
+        <v>48431</v>
+      </c>
+      <c r="M2">
+        <v>2568.25</v>
+      </c>
+      <c r="N2">
+        <v>0.2</v>
+      </c>
+      <c r="O2">
+        <v>3424.29</v>
+      </c>
+      <c r="P2">
+        <v>64205.45</v>
+      </c>
+      <c r="Q2">
+        <v>85607.26</v>
+      </c>
+      <c r="R2">
+        <v>64201.14</v>
+      </c>
+      <c r="S2">
+        <v>210.85059999999999</v>
+      </c>
+      <c r="T2">
+        <v>0.25</v>
+      </c>
+      <c r="U2">
+        <v>-2844564.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2909</v>
+      </c>
+      <c r="C3">
+        <v>3417017</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>3723123</v>
+      </c>
+      <c r="F3">
+        <v>385780</v>
+      </c>
+      <c r="G3">
+        <v>12577</v>
+      </c>
+      <c r="H3">
+        <v>48434</v>
+      </c>
+      <c r="I3">
+        <v>64579</v>
+      </c>
+      <c r="J3">
+        <v>64579</v>
+      </c>
+      <c r="K3">
+        <v>48434</v>
+      </c>
+      <c r="L3">
+        <v>47810</v>
+      </c>
+      <c r="M3">
+        <v>2573.5700000000002</v>
+      </c>
+      <c r="N3">
+        <v>38.46</v>
+      </c>
+      <c r="O3">
+        <v>3424.29</v>
+      </c>
+      <c r="P3">
+        <v>64205.440000000002</v>
+      </c>
+      <c r="Q3">
+        <v>85607.26</v>
+      </c>
+      <c r="R3">
+        <v>63377.77</v>
+      </c>
+      <c r="S3">
+        <v>170.68</v>
+      </c>
+      <c r="T3">
+        <v>0.25</v>
+      </c>
+      <c r="U3">
+        <v>-2300576.81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2697</v>
+      </c>
+      <c r="C4">
+        <v>3555953</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>3474229</v>
+      </c>
+      <c r="F4">
+        <v>4632</v>
+      </c>
+      <c r="G4">
+        <v>11736</v>
+      </c>
+      <c r="H4">
+        <v>46948</v>
+      </c>
+      <c r="I4">
+        <v>62597</v>
+      </c>
+      <c r="J4">
+        <v>62597</v>
+      </c>
+      <c r="K4">
+        <v>46948</v>
+      </c>
+      <c r="L4">
+        <v>46949</v>
+      </c>
+      <c r="M4">
+        <v>2489.41</v>
+      </c>
+      <c r="N4">
+        <v>-0.08</v>
+      </c>
+      <c r="O4">
+        <v>3319.22</v>
+      </c>
+      <c r="P4">
+        <v>62235.44</v>
+      </c>
+      <c r="Q4">
+        <v>82980.59</v>
+      </c>
+      <c r="R4">
+        <v>62237.16</v>
+      </c>
+      <c r="S4">
+        <v>193.3271</v>
+      </c>
+      <c r="T4">
+        <v>0.25</v>
+      </c>
+      <c r="U4">
+        <v>-2528140.56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>2512</v>
+      </c>
+      <c r="C5">
+        <v>3578632</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>3504009</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>11837</v>
+      </c>
+      <c r="H5">
+        <v>47346</v>
+      </c>
+      <c r="I5">
+        <v>63129</v>
+      </c>
+      <c r="J5">
+        <v>63129</v>
+      </c>
+      <c r="K5">
+        <v>47346</v>
+      </c>
+      <c r="L5">
+        <v>47346</v>
+      </c>
+      <c r="M5">
+        <v>2510.5500000000002</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>3347.4</v>
+      </c>
+      <c r="P5">
+        <v>62763.66</v>
+      </c>
+      <c r="Q5">
+        <v>83684.88</v>
+      </c>
+      <c r="R5">
+        <v>62763.66</v>
+      </c>
+      <c r="S5">
+        <v>144.65870000000001</v>
+      </c>
+      <c r="T5">
+        <v>0.25</v>
+      </c>
+      <c r="U5">
+        <v>-1907751.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9FD5A2-21A2-406E-943D-AF395A44688E}">
+  <dimension ref="A1:U5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3071</v>
+      </c>
+      <c r="C2">
+        <v>3677688</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>3404304</v>
+      </c>
+      <c r="F2">
+        <v>4761</v>
+      </c>
+      <c r="G2">
+        <v>11500</v>
+      </c>
+      <c r="H2">
+        <v>45990</v>
+      </c>
+      <c r="I2">
+        <v>61320</v>
+      </c>
+      <c r="J2">
+        <v>61320</v>
+      </c>
+      <c r="K2">
+        <v>45990</v>
+      </c>
+      <c r="L2">
+        <v>45987</v>
+      </c>
+      <c r="M2">
+        <v>2438.65</v>
+      </c>
+      <c r="N2">
+        <v>0.19</v>
+      </c>
+      <c r="O2">
+        <v>3251.49</v>
+      </c>
+      <c r="P2">
+        <v>60965.52</v>
+      </c>
+      <c r="Q2">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R2">
+        <v>60961.43</v>
+      </c>
+      <c r="S2">
+        <v>210.85130000000001</v>
+      </c>
+      <c r="T2">
+        <v>0.25</v>
+      </c>
+      <c r="U2">
+        <v>-2701022.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>7115</v>
+      </c>
+      <c r="C3">
+        <v>8521096</v>
+      </c>
+      <c r="D3">
+        <v>11514</v>
+      </c>
+      <c r="E3">
+        <v>6807692</v>
+      </c>
+      <c r="F3">
+        <v>3137</v>
+      </c>
+      <c r="G3">
+        <v>22997</v>
+      </c>
+      <c r="H3">
+        <v>45990</v>
+      </c>
+      <c r="I3">
+        <v>61320</v>
+      </c>
+      <c r="J3">
+        <v>61320</v>
+      </c>
+      <c r="K3">
+        <v>45990</v>
+      </c>
+      <c r="L3">
+        <v>30658</v>
+      </c>
+      <c r="M3">
+        <v>1625.76</v>
+      </c>
+      <c r="N3">
+        <v>0.13</v>
+      </c>
+      <c r="O3">
+        <v>3251.49</v>
+      </c>
+      <c r="P3">
+        <v>40643.68</v>
+      </c>
+      <c r="Q3">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R3">
+        <v>40640.980000000003</v>
+      </c>
+      <c r="S3">
+        <v>420.29660000000001</v>
+      </c>
+      <c r="T3">
+        <v>0.5</v>
+      </c>
+      <c r="U3">
+        <v>-10768134.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>11644</v>
+      </c>
+      <c r="C4">
+        <v>13945476</v>
+      </c>
+      <c r="D4">
+        <v>25145</v>
+      </c>
+      <c r="E4">
+        <v>10211400</v>
+      </c>
+      <c r="F4">
+        <v>3730</v>
+      </c>
+      <c r="G4">
+        <v>34494</v>
+      </c>
+      <c r="H4">
+        <v>45990</v>
+      </c>
+      <c r="I4">
+        <v>61320</v>
+      </c>
+      <c r="J4">
+        <v>61320</v>
+      </c>
+      <c r="K4">
+        <v>45990</v>
+      </c>
+      <c r="L4">
+        <v>15328</v>
+      </c>
+      <c r="M4">
+        <v>812.89</v>
+      </c>
+      <c r="N4">
+        <v>0.15</v>
+      </c>
+      <c r="O4">
+        <v>3251.49</v>
+      </c>
+      <c r="P4">
+        <v>20321.84</v>
+      </c>
+      <c r="Q4">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R4">
+        <v>20318.63</v>
+      </c>
+      <c r="S4">
+        <v>591.48199999999997</v>
+      </c>
+      <c r="T4">
+        <v>0.75</v>
+      </c>
+      <c r="U4">
+        <v>-22730981.510000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>35019</v>
+      </c>
+      <c r="C5">
+        <v>41940634</v>
+      </c>
+      <c r="D5">
+        <v>113618</v>
+      </c>
+      <c r="E5">
+        <v>13614485</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>45990</v>
+      </c>
+      <c r="H5">
+        <v>45990</v>
+      </c>
+      <c r="I5">
+        <v>61320</v>
+      </c>
+      <c r="J5">
+        <v>61320</v>
+      </c>
+      <c r="K5">
+        <v>45990</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>3251.49</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>81287.360000000001</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1586.3235999999999</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>-81284720.049999997</v>
       </c>
     </row>
   </sheetData>
@@ -6628,22 +9266,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE92C99-763D-4266-A92E-E8FFFC9475FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A182E3C1-1DE0-4E2D-A275-59BAF2F28188}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6660,7 +9298,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6677,7 +9315,7 @@
         <v>-1.79</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6694,7 +9332,7 @@
         <v>-0.87</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -6711,7 +9349,7 @@
         <v>-2.1800000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -6734,14 +9372,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7766F6-4451-4959-B235-348E84E5D72B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3994EE63-FF7E-4BE9-8C95-C0000164ECAD}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6767,7 +9405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6793,7 +9431,7 @@
         <v>-2741986.6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6819,7 +9457,7 @@
         <v>-2296535.7799999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -6845,7 +9483,7 @@
         <v>-2543875.48</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -6877,20 +9515,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE35B8B5-B6EC-4D1E-B7BB-8A9DD849FFC8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9560C2C8-3E21-4FBE-B651-EC05B97A277C}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6916,7 +9554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6942,7 +9580,7 @@
         <v>-8339592.2800000003</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6968,7 +9606,7 @@
         <v>-15742760.09</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -6994,7 +9632,7 @@
         <v>-27788443.390000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -7026,14 +9664,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F139C7D-7C91-42B0-896A-470227B3287A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869D2B3A-D029-4B02-AF50-659667B9D01A}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7059,7 +9697,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7085,7 +9723,7 @@
         <v>-66.068299999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7111,7 +9749,7 @@
         <v>-140.63720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -7137,7 +9775,7 @@
         <v>-52.133899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -7169,14 +9807,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB8AAE9-0D53-4706-B083-9238A8122934}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60BA737-6FAC-411D-92EA-DBD204F42411}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7202,7 +9840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7228,7 +9866,7 @@
         <v>-66.068299999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7254,7 +9892,7 @@
         <v>-140.63720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -7280,7 +9918,7 @@
         <v>-52.133899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -7312,25 +9950,25 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3C9C43-10BB-4347-ACE4-7D7A1E581318}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEAD2990-8185-4DED-9CE4-009A477E090C}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="16.90625" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" customWidth="1"/>
-    <col min="8" max="8" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7356,7 +9994,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7382,7 +10020,7 @@
         <v>-66.068299999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -7408,7 +10046,7 @@
         <v>-140.63720000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -7434,7 +10072,7 @@
         <v>-52.133899999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>

</xml_diff>